<commit_message>
update terminology and workflow chart
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29E39DB-FBF1-43BF-B84A-8A473BE82389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508906E6-2779-422C-AB35-E2074D74E5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Term</t>
   </si>
@@ -292,9 +292,6 @@
     <t>Privacy</t>
   </si>
   <si>
-    <t>The recorded factual material commonly accepted in the scientific community as necessary to validate research findings (OMB Circular A-110).</t>
-  </si>
-  <si>
     <t>Identifying information was never collected. This data can not be linked across time or measures.</t>
   </si>
   <si>
@@ -368,6 +365,42 @@
   </si>
   <si>
     <t>Data collected from a study where researchers are observing the effect of an intervention without manipulating who is exposed to the intervention. This includes many formats that education researchers collect data with (ex: survey, observation, assessment).</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>A classification that specifies what types of values are contained in a variable and what kinds of operations can be performed on that variable. Examples of types include numeric, character, logical, or datetime.</t>
+  </si>
+  <si>
+    <t>variable format, variable class</t>
+  </si>
+  <si>
+    <t>The recorded factual material commonly accepted in the scientific community as necessary to validate research findings. (OMB Circular A-110)</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>The Common Rule definition of research is a systematic investigation, including research development, testing, and evaluation, designed to develop or contribute to generalizable knowledge.</t>
+  </si>
+  <si>
+    <t>Primary Data</t>
+  </si>
+  <si>
+    <t>Secondary Data</t>
+  </si>
+  <si>
+    <t>extant data</t>
+  </si>
+  <si>
+    <t>original data</t>
+  </si>
+  <si>
+    <t>First hand data that is generated/collected by the research team as part of the research study.</t>
+  </si>
+  <si>
+    <t>Existing data generated/collected by external organizations such as governments at an earlier point in time.</t>
   </si>
 </sst>
 </file>
@@ -719,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFDD66-17FF-4EA8-972E-A7EADB2C89E2}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,10 +852,10 @@
         <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -830,7 +863,7 @@
         <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -838,18 +871,18 @@
         <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -876,7 +909,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -996,7 +1029,7 @@
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1007,7 +1040,7 @@
         <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1026,7 +1059,7 @@
         <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1034,7 +1067,7 @@
         <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,18 +1115,18 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s">
         <v>102</v>
-      </c>
-      <c r="C38" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,7 +1134,7 @@
         <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1109,7 +1142,7 @@
         <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1120,7 +1153,7 @@
         <v>35</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1128,31 +1161,72 @@
         <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update checklists, integrate feedback
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3129CA75-C441-4389-B508-B96E6E69AD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E62038-A53D-4C54-95BD-895D63AB0AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="790" windowWidth="19420" windowHeight="11620" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -316,9 +316,6 @@
     <t>Personally identifiable information (PII) in your data has been removed and names are replaced with a code and the only way to link the data back to an individual is through that code. The identifying code file (linking key) is stored separate from the research data.</t>
   </si>
   <si>
-    <t>study roster, demographic file, master list, master key, linking key, code key, key code, main list, identifiers dataset, crosswalk, record keeping, tracking, participant tracking</t>
-  </si>
-  <si>
     <t>Data that includes personally identifiable information.</t>
   </si>
   <si>
@@ -401,6 +398,9 @@
   </si>
   <si>
     <t>measurement unit, variable format, variable class</t>
+  </si>
+  <si>
+    <t>study roster, master list, master key, linking key, code key, key code, main list, identifiers dataset, crosswalk, record keeping, tracking, participant tracking</t>
   </si>
 </sst>
 </file>
@@ -754,18 +754,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFDD66-17FF-4EA8-972E-A7EADB2C89E2}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
+    <col min="2" max="2" width="39.26953125" customWidth="1"/>
+    <col min="3" max="3" width="35.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -784,7 +784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -795,7 +795,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -806,7 +806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -814,7 +814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -825,7 +825,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -836,7 +836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -847,7 +847,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -858,7 +858,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -866,7 +866,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -877,15 +877,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -893,7 +893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -904,18 +904,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -923,7 +923,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -931,7 +931,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -939,7 +939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -947,7 +947,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -958,7 +958,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -969,7 +969,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -980,7 +980,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -991,7 +991,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1029,10 +1029,10 @@
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1040,10 +1040,10 @@
         <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1059,18 +1059,18 @@
         <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1113,31 +1113,31 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>100</v>
       </c>
-      <c r="C37" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C38" t="s">
         <v>101</v>
       </c>
-      <c r="C38" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -1153,10 +1153,10 @@
         <v>35</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -1164,69 +1164,69 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>103</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>104</v>
-      </c>
-      <c r="C44" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" t="s">
         <v>110</v>
       </c>
-      <c r="B46" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" t="s">
         <v>113</v>
       </c>
-      <c r="C47" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>115</v>
       </c>
-      <c r="B48" t="s">
-        <v>118</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B49" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>116</v>
-      </c>
-      <c r="B49" t="s">
-        <v>117</v>
-      </c>
-      <c r="C49" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revise small part of data dictionary, revise citations
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E62038-A53D-4C54-95BD-895D63AB0AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292B8786-E1D9-4D03-A13C-58D97C674EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -52,9 +51,6 @@
     <t>a single funded research project resulting in one more more datasets to be used to answer a research question.</t>
   </si>
   <si>
-    <t>Randomized Controlled Trial</t>
-  </si>
-  <si>
     <t>RCT</t>
   </si>
   <si>
@@ -250,9 +246,6 @@
     <t>Qualitative data</t>
   </si>
   <si>
-    <t>Non-numeric data typically made up of text, images, video or other artifacts.</t>
-  </si>
-  <si>
     <t>Quantitative data</t>
   </si>
   <si>
@@ -298,12 +291,6 @@
     <t>pseudonymisation, coded data, indirectly identifiable</t>
   </si>
   <si>
-    <t>Privacy concerns people. Ensuring others are given control to the access of themselves and their information.</t>
-  </si>
-  <si>
-    <t>Confidentiality concerns data. Ensuring participants agree to how their private and identifable information will be managed and disseminated.</t>
-  </si>
-  <si>
     <t>Identifiable data</t>
   </si>
   <si>
@@ -334,24 +321,9 @@
     <t>The transfer of data to a facility, such as a repository, that preserves and stores data long-term.</t>
   </si>
   <si>
-    <t>Observational Data</t>
-  </si>
-  <si>
-    <t>Experimental Data</t>
-  </si>
-  <si>
     <t>Data collected from a study where researchers randomly introduce an intervention and study the effects.</t>
   </si>
   <si>
-    <t>Simulation Data</t>
-  </si>
-  <si>
-    <t>Derived Data</t>
-  </si>
-  <si>
-    <t>Extant Data</t>
-  </si>
-  <si>
     <t>Data created through transformations of existing data.</t>
   </si>
   <si>
@@ -379,12 +351,6 @@
     <t>The Common Rule definition of research is a systematic investigation, including research development, testing, and evaluation, designed to develop or contribute to generalizable knowledge.</t>
   </si>
   <si>
-    <t>Primary Data</t>
-  </si>
-  <si>
-    <t>Secondary Data</t>
-  </si>
-  <si>
     <t>extant data</t>
   </si>
   <si>
@@ -401,6 +367,39 @@
   </si>
   <si>
     <t>study roster, master list, master key, linking key, code key, key code, main list, identifiers dataset, crosswalk, record keeping, tracking, participant tracking</t>
+  </si>
+  <si>
+    <t>Confidentiality concerns data, ensuring participants agree to how their private and identifable information will be managed and disseminated.</t>
+  </si>
+  <si>
+    <t>Observational data</t>
+  </si>
+  <si>
+    <t>Experimental data</t>
+  </si>
+  <si>
+    <t>Simulation data</t>
+  </si>
+  <si>
+    <t>Derived data</t>
+  </si>
+  <si>
+    <t>Primary data</t>
+  </si>
+  <si>
+    <t>Secondary data</t>
+  </si>
+  <si>
+    <t>Extant data</t>
+  </si>
+  <si>
+    <t>Randomized controlled trial</t>
+  </si>
+  <si>
+    <t>Privacy concerns people, ensuring they are given control to the access of themselves and their information.</t>
+  </si>
+  <si>
+    <t>Non-numeric data typically made up of text, images, video, or other artifacts.</t>
   </si>
 </sst>
 </file>
@@ -754,18 +753,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFDD66-17FF-4EA8-972E-A7EADB2C89E2}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1796875" customWidth="1"/>
-    <col min="2" max="2" width="39.26953125" customWidth="1"/>
-    <col min="3" max="3" width="35.26953125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -776,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -784,449 +783,449 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>82</v>
       </c>
-      <c r="B9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="C40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>81</v>
       </c>
-      <c r="B11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>102</v>
-      </c>
-      <c r="C43" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>109</v>
-      </c>
-      <c r="B46" t="s">
-        <v>120</v>
-      </c>
-      <c r="C46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>114</v>
-      </c>
-      <c r="B48" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>115</v>
-      </c>
-      <c r="B49" t="s">
-        <v>116</v>
-      </c>
-      <c r="C49" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move glossary, add many edits
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292B8786-E1D9-4D03-A13C-58D97C674EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF223F78-10E0-48D3-89CA-4C0CA97F65B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t>Term</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Study</t>
   </si>
   <si>
-    <t>a single funded research project resulting in one more more datasets to be used to answer a research question.</t>
-  </si>
-  <si>
     <t>RCT</t>
   </si>
   <si>
@@ -99,18 +96,6 @@
     <t>PII</t>
   </si>
   <si>
-    <t>Personally identifiable information is protected information that can directly or indirectly identify a study participant. It includes but is not limited to name, social security number, email, birthdate, district or school name.</t>
-  </si>
-  <si>
-    <t>Study ID</t>
-  </si>
-  <si>
-    <t>participant ID, location ID, site ID, unique identifier (UID), subject ID, participant code, record id</t>
-  </si>
-  <si>
-    <t>This is a numeric or alphanumeric identifier that is unique to every participant, site or object in order to create confidential and de-identified data. These identifiers allow researchers to link data across time or measure.</t>
-  </si>
-  <si>
     <t>Participant database</t>
   </si>
   <si>
@@ -153,9 +138,6 @@
     <t>dataframe, spreadsheet</t>
   </si>
   <si>
-    <t>A structured collection of data usually stored in tabular form. A research study usually produces one final dataset per entity/unit (ex: teacher dataset, student dataset).</t>
-  </si>
-  <si>
     <t>Raw data</t>
   </si>
   <si>
@@ -171,9 +153,6 @@
     <t>processed data</t>
   </si>
   <si>
-    <t>Any data that has been manipulated or modified.</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
@@ -216,9 +195,6 @@
     <t>file path</t>
   </si>
   <si>
-    <t>file structure</t>
-  </si>
-  <si>
     <t>Standardization</t>
   </si>
   <si>
@@ -297,18 +273,9 @@
     <t xml:space="preserve">Identifying information has been removed or distorted and the data can no longer be re-associated with the underlying individual (the linking key no longer exists). </t>
   </si>
   <si>
-    <t>anonymized data</t>
-  </si>
-  <si>
-    <t>Personally identifiable information (PII) in your data has been removed and names are replaced with a code and the only way to link the data back to an individual is through that code. The identifying code file (linking key) is stored separate from the research data.</t>
-  </si>
-  <si>
     <t>Data that includes personally identifiable information.</t>
   </si>
   <si>
-    <t>Combining datasets together in a side by side manner (matching on an identifier).</t>
-  </si>
-  <si>
     <t>A cataloging structure for files and folders on your computer.</t>
   </si>
   <si>
@@ -324,21 +291,9 @@
     <t>Data collected from a study where researchers randomly introduce an intervention and study the effects.</t>
   </si>
   <si>
-    <t>Data created through transformations of existing data.</t>
-  </si>
-  <si>
     <t>Data generated through imitations of a real-world process using computer models.</t>
   </si>
   <si>
-    <t>Existing data sources created from external to the research team/study.</t>
-  </si>
-  <si>
-    <t>Data collected from a study where researchers are observing the effect of an intervention without manipulating who is exposed to the intervention. This includes many formats that education researchers collect data with (ex: survey, observation, assessment).</t>
-  </si>
-  <si>
-    <t>Data Type</t>
-  </si>
-  <si>
     <t>A classification that specifies what types of values are contained in a variable and what kinds of operations can be performed on that variable. Examples of types include numeric, character, logical, or datetime.</t>
   </si>
   <si>
@@ -348,27 +303,15 @@
     <t>Research</t>
   </si>
   <si>
-    <t>The Common Rule definition of research is a systematic investigation, including research development, testing, and evaluation, designed to develop or contribute to generalizable knowledge.</t>
-  </si>
-  <si>
-    <t>extant data</t>
-  </si>
-  <si>
     <t>original data</t>
   </si>
   <si>
     <t>First hand data that is generated/collected by the research team as part of the research study.</t>
   </si>
   <si>
-    <t>Existing data generated/collected by external organizations such as governments at an earlier point in time.</t>
-  </si>
-  <si>
     <t>measurement unit, variable format, variable class</t>
   </si>
   <si>
-    <t>study roster, master list, master key, linking key, code key, key code, main list, identifiers dataset, crosswalk, record keeping, tracking, participant tracking</t>
-  </si>
-  <si>
     <t>Confidentiality concerns data, ensuring participants agree to how their private and identifable information will be managed and disseminated.</t>
   </si>
   <si>
@@ -387,9 +330,6 @@
     <t>Primary data</t>
   </si>
   <si>
-    <t>Secondary data</t>
-  </si>
-  <si>
     <t>Extant data</t>
   </si>
   <si>
@@ -400,6 +340,123 @@
   </si>
   <si>
     <t>Non-numeric data typically made up of text, images, video, or other artifacts.</t>
+  </si>
+  <si>
+    <t>Raw data that has been manipulated or modified for the purposes of correcting and clarifying information.</t>
+  </si>
+  <si>
+    <t>The status of this data is protected. Personally identifiable information (PII) in your data has been removed and names are replaced with a code and the only way to link the data back to an individual is through that code. The identifying code file (linking key) is stored separate from the research data.</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>Data created through transformations of existing data (e.g., mean scores).</t>
+  </si>
+  <si>
+    <t>A structured collection of data usually stored in tabular form. A research study usually produces one final dataset per entity/unit (e.g., teacher dataset, student dataset).</t>
+  </si>
+  <si>
+    <t>Direct identifiers</t>
+  </si>
+  <si>
+    <t>These identifiers can directly identify a participant and should always be removed from research study data. There should be no need to keep these identifiers for analysis (i.e. name, email, address).</t>
+  </si>
+  <si>
+    <t>file structure, file tree</t>
+  </si>
+  <si>
+    <t>secondary data</t>
+  </si>
+  <si>
+    <t>Indirect identifiers</t>
+  </si>
+  <si>
+    <t>Even though these identifiers are not necessarily uniquely tied to one individual (i.e., birthdate or place of birth), if combined, this information could indirectly identify a participant. Therefore this information should be managed before publicly sharing data.</t>
+  </si>
+  <si>
+    <t>Combining datasets together in a side by side manner (matching on one or more unique identifiers).</t>
+  </si>
+  <si>
+    <t>Data collected from a study where researchers are observing the effect of an intervention without manipulating who is exposed to the intervention. This includes many formats that education researchers collect data with (e.g., survey, observation, assessment).</t>
+  </si>
+  <si>
+    <t>study roster, master list, master key, linking key, tracking database</t>
+  </si>
+  <si>
+    <t>Personally identifiable information</t>
+  </si>
+  <si>
+    <t>This includes direct identifiers (e.g., name and email), as well as indirect identifiers that, if combined with other variables, could identify a participant (e.g., full birthdate and county of residence). Under FERPA, additional PII, such as a district or school ID, should also be removed. Protected health identifiers (PHI) is a similar protected category of information. There are 18 HIPAA protected health identifiers that should be removed from data in order to meet the Safe Harbor de-identification method (e.g., name, email, address).</t>
+  </si>
+  <si>
+    <t>Private data</t>
+  </si>
+  <si>
+    <t>The Common Rule (45 CFR 46) definition of research is a systematic investigation, including research development, testing, and evaluation, designed to develop or contribute to generalizable knowledge.</t>
+  </si>
+  <si>
+    <t>Existing data generated/collected by external organizations such as governments at an earlier point in time (e.g., administrative data).</t>
+  </si>
+  <si>
+    <t>Sensitive data</t>
+  </si>
+  <si>
+    <t>Private information that could cause harm and should be protected from unwarranted disclosure.</t>
+  </si>
+  <si>
+    <t>Highly restricted data with limited access (i.e., passwords).</t>
+  </si>
+  <si>
+    <t>This is a numeric or alphanumeric identifier that is unique to every participant or site in order to create confidential and de-identified data. These identifiers allow researchers to link data across time or measure.</t>
+  </si>
+  <si>
+    <t>HIPAA</t>
+  </si>
+  <si>
+    <t>FERPA</t>
+  </si>
+  <si>
+    <t>anonymized data, anonymization</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Measure</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>A means used to collect data using an instrument (e.g., a paper form, an online survey platform)</t>
+  </si>
+  <si>
+    <t>A mechanism designed to collect original data (e.g., observation form, questionnaire, assessment)</t>
+  </si>
+  <si>
+    <t>In this book, I use the term measure broadly to refer to a collection of items used to measure an outcome (e.g., an existing scale, an existing academic assessment).</t>
+  </si>
+  <si>
+    <t>Similar to the term "measure", this is a collection of items used to measure an outcome. However, I typically use this term to more specifically refer to questionnaires that have had psychometric properties assessed. Scales may also be made up of subscales (i.e., groupings of items).</t>
+  </si>
+  <si>
+    <t>The Health Insurance Portability and Accountability Act is a federal law covering the protection of sensitive health information.</t>
+  </si>
+  <si>
+    <t>The Family Educational Rights and Privacy Act is a federal law governing the disclosure of personally identifiable information in education records (e.g., name, address, DOB). The law applies to all public elementary and secondary schools, as well as post-secondary institutions.</t>
+  </si>
+  <si>
+    <t>Unique participant identifier</t>
+  </si>
+  <si>
+    <t>study ID, site ID, unique identifier (UID), subject ID, participant code, record id</t>
+  </si>
+  <si>
+    <t>A single funded research project resulting in one or more datasets to be used to answer a research question.</t>
   </si>
 </sst>
 </file>
@@ -751,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFDD66-17FF-4EA8-972E-A7EADB2C89E2}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,458 +834,536 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>127</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>116</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>116</v>
-      </c>
-      <c r="B48" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>117</v>
-      </c>
-      <c r="B49" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>138</v>
+      </c>
+      <c r="B55" t="s">
+        <v>139</v>
+      </c>
+      <c r="C55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C58">
+    <sortCondition ref="A2:A58"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update citations and wording in a few spots of the documentation chapter
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF223F78-10E0-48D3-89CA-4C0CA97F65B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9F5EC1-98E5-4B10-B6EF-A348A513057F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
   <si>
     <t>Term</t>
   </si>
@@ -457,6 +457,18 @@
   </si>
   <si>
     <t>A single funded research project resulting in one or more datasets to be used to answer a research question.</t>
+  </si>
+  <si>
+    <t>A dataset in which 15 of the 18 HIPAA protected identifiers have been removed. Age, dates, and city/state/zipcode can remain.</t>
+  </si>
+  <si>
+    <t>Limited data set</t>
+  </si>
+  <si>
+    <t>A dataset that contains sensitive, confidential, or proprietary information.</t>
+  </si>
+  <si>
+    <t>Restricted-use data</t>
   </si>
 </sst>
 </file>
@@ -808,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFDD66-17FF-4EA8-972E-A7EADB2C89E2}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,297 +1084,313 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>142</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
       <c r="C30" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>97</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>99</v>
-      </c>
-      <c r="B41" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="C46" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="C48" t="s">
-        <v>85</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="C49" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C50" t="s">
-        <v>140</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>131</v>
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="C54" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>138</v>
-      </c>
-      <c r="B55" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="C56" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="C57" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>10</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>11</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C58">
-    <sortCondition ref="A2:A58"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
+    <sortCondition ref="A2:A60"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Several revisions to data structure chapter, as well as DMP and storage
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23165C6-76EC-410B-BEF5-4650F349AAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97218B41-1BEB-4CA5-9FAA-23144C3855E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
@@ -297,9 +297,6 @@
     <t>measurement unit, variable format, variable class</t>
   </si>
   <si>
-    <t>Confidentiality concerns data, ensuring participants agree to how their private and identifable information will be managed and disseminated.</t>
-  </si>
-  <si>
     <t>Observational data</t>
   </si>
   <si>
@@ -351,9 +348,6 @@
     <t>Combining datasets together in a side by side manner (matching on one or more unique identifiers).</t>
   </si>
   <si>
-    <t>Data collected from a study where researchers are observing the effect of an intervention without manipulating who is exposed to the intervention. This includes many formats that education researchers collect data with (e.g., survey, observation, assessment).</t>
-  </si>
-  <si>
     <t>study roster, master list, master key, linking key, tracking database</t>
   </si>
   <si>
@@ -508,6 +502,12 @@
   </si>
   <si>
     <t>The Common Rule (45 CFR 46) definition of a human subject is a living individual about whom an investigator conducting research obtains; 1) Data through intervention or interaction with the individual, or 2) identifiable private information.</t>
+  </si>
+  <si>
+    <t>Data collected from a study where researchers are observing the effect of an intervention without manipulating who is exposed to the intervention.</t>
+  </si>
+  <si>
+    <t>Confidentiality concerns data, ensuring participants agree to how their private and identifiable information will be managed and disseminated.</t>
   </si>
 </sst>
 </file>
@@ -543,9 +543,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,7 +862,7 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,12 +891,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>151</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,7 +931,7 @@
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,13 +944,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -959,7 +958,7 @@
         <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,7 +966,7 @@
         <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -975,7 +974,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1002,7 +1001,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
         <v>86</v>
@@ -1027,10 +1026,10 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1038,7 +1037,7 @@
         <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
         <v>73</v>
@@ -1046,18 +1045,18 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1065,7 +1064,7 @@
         <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
         <v>75</v>
@@ -1073,7 +1072,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
         <v>79</v>
@@ -1081,21 +1080,21 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,18 +1107,18 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1132,26 +1131,26 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1164,10 +1163,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,7 +1177,7 @@
         <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1191,10 +1190,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1202,7 +1201,7 @@
         <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C37" t="s">
         <v>19</v>
@@ -1221,18 +1220,18 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
         <v>84</v>
@@ -1246,26 +1245,26 @@
         <v>70</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>144</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1273,7 +1272,7 @@
         <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1286,7 +1285,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
@@ -1327,50 +1326,50 @@
         <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>148</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C52" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C54" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C55" t="s">
         <v>80</v>
@@ -1389,7 +1388,7 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1416,10 +1415,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1435,13 +1434,13 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1449,7 +1448,7 @@
         <v>39</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C63" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
draft of data sharing
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97218B41-1BEB-4CA5-9FAA-23144C3855E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302FCB41-DB77-46FB-B005-BC05652F3227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
   <si>
     <t>Term</t>
   </si>
@@ -405,9 +405,6 @@
     <t>Unique participant identifier</t>
   </si>
   <si>
-    <t>study ID, site ID, unique identifier (UID), subject ID, participant code, record id</t>
-  </si>
-  <si>
     <t>A single funded research project resulting in one or more datasets to be used to answer a research question.</t>
   </si>
   <si>
@@ -438,9 +435,6 @@
     <t xml:space="preserve">These variables are unique to an individual and can be used to directly identify a participant (e.g., name, email address). </t>
   </si>
   <si>
-    <t>These variables do not alone identify a particular individual (e.g., ethnicity, gender), but if combined with other information or if category numbers are small, they could be used to identify a participant</t>
-  </si>
-  <si>
     <t>Coded data</t>
   </si>
   <si>
@@ -508,6 +502,21 @@
   </si>
   <si>
     <t>Confidentiality concerns data, ensuring participants agree to how their private and identifiable information will be managed and disseminated.</t>
+  </si>
+  <si>
+    <t>quasi-identifiers</t>
+  </si>
+  <si>
+    <t>These variables do not alone identify a particular individual (e.g., ethnicity, gender), but if combined with other information, they could be used to identify a participant</t>
+  </si>
+  <si>
+    <t>study ID, site ID, unique identifier (UID), subject ID, participant code, record id, proxy ID</t>
+  </si>
+  <si>
+    <t>Disclosure risk</t>
+  </si>
+  <si>
+    <t>The risk of re-identifying a participant and the harm that may come from that disclosure.</t>
   </si>
 </sst>
 </file>
@@ -859,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFDD66-17FF-4EA8-972E-A7EADB2C89E2}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,10 +902,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -944,13 +953,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,7 +967,7 @@
         <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -966,7 +975,7 @@
         <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -974,7 +983,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1026,7 +1035,7 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
         <v>99</v>
@@ -1037,7 +1046,7 @@
         <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
         <v>73</v>
@@ -1056,7 +1065,7 @@
         <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1072,413 +1081,424 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>127</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>102</v>
+      </c>
+      <c r="B30" t="s">
+        <v>156</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="C34" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>156</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>153</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>91</v>
+      </c>
+      <c r="B41" t="s">
+        <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="C42" t="s">
-        <v>151</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>141</v>
-      </c>
-      <c r="B43" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>139</v>
+      </c>
+      <c r="B44" t="s">
+        <v>135</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>31</v>
+      </c>
+      <c r="B48" t="s">
+        <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>126</v>
-      </c>
-      <c r="B51" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>140</v>
+        <v>125</v>
+      </c>
+      <c r="B52" t="s">
+        <v>129</v>
       </c>
       <c r="C52" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>108</v>
-      </c>
-      <c r="B53" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C53" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>145</v>
       </c>
       <c r="C54" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="C55" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>54</v>
+      </c>
+      <c r="B60" t="s">
+        <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="C61" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="C62" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C63" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="C64" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" t="s">
+        <v>42</v>
+      </c>
+      <c r="C65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>10</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>11</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C65">
-    <sortCondition ref="A2:A65"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C66">
+    <sortCondition ref="A2:A66"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Change data structure chapter name, make edits throughout
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31566D3-5CA7-4A18-A89E-455479C02312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBF0FCE-3401-45F0-B603-773EC2468CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
   <si>
     <t>Term</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>experiment</t>
-  </si>
-  <si>
     <t>The individual or group receives the intervention.</t>
   </si>
   <si>
@@ -102,12 +99,6 @@
     <t>The loss of study units from the sample, often seen in longitudinal studies.</t>
   </si>
   <si>
-    <t>Longitudinal</t>
-  </si>
-  <si>
-    <t>Data is collected on participants over a period of time.</t>
-  </si>
-  <si>
     <t>Cross-sectional</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>File formats</t>
   </si>
   <si>
-    <t>Education research data is typically collected in one of three file formats: text( .txt, .pdf, .docx), tabular (.xlsx, .csv, .sav) , multimedia (.mpeg, .wav).</t>
-  </si>
-  <si>
     <t>Dataset</t>
   </si>
   <si>
@@ -183,18 +171,9 @@
     <t>file path</t>
   </si>
   <si>
-    <t>Standardization</t>
-  </si>
-  <si>
-    <t>Developing a set of agreed upon technical standards and applying them within and across all research projects.</t>
-  </si>
-  <si>
     <t>Merge</t>
   </si>
   <si>
-    <t>join, link</t>
-  </si>
-  <si>
     <t>Append</t>
   </si>
   <si>
@@ -285,9 +264,6 @@
     <t>Research</t>
   </si>
   <si>
-    <t>original data</t>
-  </si>
-  <si>
     <t>First hand data that is generated/collected by the research team as part of the research study.</t>
   </si>
   <si>
@@ -303,9 +279,6 @@
     <t>Derived data</t>
   </si>
   <si>
-    <t>Primary data</t>
-  </si>
-  <si>
     <t>Extant data</t>
   </si>
   <si>
@@ -339,9 +312,6 @@
     <t>Indirect identifiers</t>
   </si>
   <si>
-    <t>Combining datasets together in a side by side manner (matching on one or more unique identifiers).</t>
-  </si>
-  <si>
     <t>study roster, master list, master key, linking key, tracking database</t>
   </si>
   <si>
@@ -459,9 +429,6 @@
     <t>An umbrella term that encompasses proprietary, ethical, contractual, or private information that should be protected from unwarranted disclosure. There are varying levels of data sensitivity.</t>
   </si>
   <si>
-    <t>Under the HIPAA Privacy Rule, a limited datasest is one in which 16 of the 18 HIPAA protected identifiers have been removed. Age, dates, and city/state/zipcode can remain. A limited dataset may be disclosed to external parties without authorization for specified purposes and often a data use agreement is required. This dataset is not considered de-identified and must be safeguarded against unauthorized access.</t>
-  </si>
-  <si>
     <t>A dataset that cannot be publicly released due to containing sensitive information or a combination of variables that could enable identification. These data require controlled access conditions and may be shared through data use agreements or other application processes.</t>
   </si>
   <si>
@@ -480,9 +447,6 @@
     <t>Highly restricted and typically not publicly shared, or is shared with limited access (i.e., passwords, illegal behaviors, medical records, financial information).</t>
   </si>
   <si>
-    <t>data set, dataframe, spreadsheet, rectangular data, tabular data</t>
-  </si>
-  <si>
     <t>This includes direct identifiers (e.g., name and email), as well as indirect identifiers that, if combined with other variables or if in small enough numbers, could identify a participant (e.g., full birthdate and place of birth).</t>
   </si>
   <si>
@@ -504,9 +468,6 @@
     <t>These variables do not alone identify a particular individual (e.g., ethnicity, gender), but if combined with other information, they could be used to identify a participant</t>
   </si>
   <si>
-    <t>study ID, site ID, unique identifier (UID), subject ID, participant code, record id, proxy ID</t>
-  </si>
-  <si>
     <t>Disclosure risk</t>
   </si>
   <si>
@@ -520,6 +481,87 @@
   </si>
   <si>
     <t>A storage location for researchers to deposit data and supporting materials associated with their research.</t>
+  </si>
+  <si>
+    <t>study ID, site ID, unique identifier (UID), subject ID, participant code, record ID</t>
+  </si>
+  <si>
+    <t>Primary key</t>
+  </si>
+  <si>
+    <t>Original data</t>
+  </si>
+  <si>
+    <t>primary data</t>
+  </si>
+  <si>
+    <t>One or more variables that uniquely define rows in your data</t>
+  </si>
+  <si>
+    <t>Foreign key</t>
+  </si>
+  <si>
+    <t>One or more variables associated with unique values in another table</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>Normalize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this book, the term normalize is used to refer to returning a value to its normal, or expected state </t>
+  </si>
+  <si>
+    <t>Standardize</t>
+  </si>
+  <si>
+    <t>Developing and implementing a set of consistent procedures</t>
+  </si>
+  <si>
+    <t>Database design</t>
+  </si>
+  <si>
+    <t>A collection of decisions regarding how tables, or datasets, will be organized and related to one another</t>
+  </si>
+  <si>
+    <t>data set, dataframe, spreadsheet, rectangular data, tabular data, table</t>
+  </si>
+  <si>
+    <t>Data structure</t>
+  </si>
+  <si>
+    <t>database schema, data modeling</t>
+  </si>
+  <si>
+    <t>repeated measures</t>
+  </si>
+  <si>
+    <t>A way of organizing data to allow for more efficient processing and storage. In particular, repeated measures data can be structured in either long or wide format.</t>
+  </si>
+  <si>
+    <t>The same information is collected from the same subjects at multiple time points.</t>
+  </si>
+  <si>
+    <t>Longitudinal data</t>
+  </si>
+  <si>
+    <t>calculated values</t>
+  </si>
+  <si>
+    <t>vertical join, join columns</t>
+  </si>
+  <si>
+    <t>horizontal join, join rows, link</t>
+  </si>
+  <si>
+    <t>Under the HIPAA Privacy Rule, a limited datasest is one in which 16 of the 18 HIPAA protected identifiers have been removed. Age, dates, and city/state/ZIP Code can remain. A limited dataset may be disclosed to external parties without authorization for specified purposes and often a data use agreement is required. This dataset is not considered de-identified and must be safeguarded against unauthorized access.</t>
+  </si>
+  <si>
+    <t>Combining datasets together in a side-by-side manner (matching on one or more unique identifiers).</t>
+  </si>
+  <si>
+    <t>A way that information is encoded for storage on a computer. There are both proprietary (e.g., SPSS, XLSX) and non-proprietary formats (e.g., CSV, TXT).</t>
   </si>
 </sst>
 </file>
@@ -871,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFDD66-17FF-4EA8-972E-A7EADB2C89E2}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,53 +939,56 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>171</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,555 +1001,604 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" t="s">
-        <v>85</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" t="s">
         <v>88</v>
-      </c>
-      <c r="C20" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
       </c>
       <c r="C21" t="s">
-        <v>130</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B25" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>81</v>
+      </c>
+      <c r="B27" t="s">
+        <v>115</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>154</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>100</v>
-      </c>
-      <c r="B31" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>169</v>
+      </c>
+      <c r="B37" t="s">
+        <v>166</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C38" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>172</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="C41" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>151</v>
+      </c>
+      <c r="B43" t="s">
+        <v>152</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>17</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
       </c>
       <c r="C44" t="s">
-        <v>147</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>138</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>119</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>150</v>
       </c>
       <c r="C47" t="s">
-        <v>63</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>91</v>
-      </c>
-      <c r="B48" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>127</v>
+      </c>
+      <c r="B50" t="s">
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>27</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
       </c>
       <c r="C54" t="s">
-        <v>139</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>106</v>
-      </c>
-      <c r="B55" t="s">
-        <v>143</v>
+        <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="C57" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>3</v>
+        <v>113</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" t="s">
-        <v>6</v>
+        <v>126</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>132</v>
       </c>
       <c r="C60" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="C62" t="s">
-        <v>15</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>120</v>
-      </c>
-      <c r="B63" t="s">
-        <v>156</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C65" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>37</v>
+      </c>
+      <c r="B70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>10</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B71" t="s">
         <v>11</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C71" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C66">
-    <sortCondition ref="A2:A66"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C71">
+    <sortCondition ref="A2:A71"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update all images except for Tracking chapter, make minor edits from feedback
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBF0FCE-3401-45F0-B603-773EC2468CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DE4D39-280D-49ED-B182-FADBF65FAD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
@@ -381,9 +381,6 @@
     <t>column, field, question, data element</t>
   </si>
   <si>
-    <t>secondary data, administrative data</t>
-  </si>
-  <si>
     <t>Existing data generated/collected by external organizations at an earlier point in time (e.g., school records).</t>
   </si>
   <si>
@@ -562,6 +559,9 @@
   </si>
   <si>
     <t>A way that information is encoded for storage on a computer. There are both proprietary (e.g., SPSS, XLSX) and non-proprietary formats (e.g., CSV, TXT).</t>
+  </si>
+  <si>
+    <t>secondary data, administrative data, third-party data</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
   <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,10 +947,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
         <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
         <v>70</v>
@@ -1001,13 +1001,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,7 +1015,7 @@
         <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
         <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -1058,21 +1058,21 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" t="s">
         <v>146</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>147</v>
-      </c>
-      <c r="C15" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,13 +1099,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" t="s">
         <v>161</v>
-      </c>
-      <c r="B19" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
         <v>88</v>
@@ -1124,7 +1124,7 @@
         <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
         <v>66</v>
@@ -1135,7 +1135,7 @@
         <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C22" t="s">
         <v>87</v>
@@ -1146,7 +1146,7 @@
         <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1162,10 +1162,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" t="s">
         <v>144</v>
-      </c>
-      <c r="C25" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1181,10 +1181,10 @@
         <v>81</v>
       </c>
       <c r="B27" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" t="s">
         <v>115</v>
-      </c>
-      <c r="C27" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1200,23 +1200,23 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C30" t="s">
         <v>154</v>
-      </c>
-      <c r="C30" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" t="s">
         <v>138</v>
-      </c>
-      <c r="C31" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,10 +1240,10 @@
         <v>91</v>
       </c>
       <c r="B34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C34" t="s">
         <v>142</v>
-      </c>
-      <c r="C34" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1259,18 +1259,18 @@
         <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1286,10 +1286,10 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1302,10 +1302,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" t="s">
         <v>157</v>
-      </c>
-      <c r="C41" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1313,15 +1313,15 @@
         <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" t="s">
         <v>151</v>
-      </c>
-      <c r="B43" t="s">
-        <v>152</v>
       </c>
       <c r="C43" t="s">
         <v>76</v>
@@ -1354,18 +1354,18 @@
         <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1381,18 +1381,18 @@
         <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" t="s">
         <v>127</v>
-      </c>
-      <c r="B50" t="s">
-        <v>123</v>
-      </c>
-      <c r="C50" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1462,18 +1462,18 @@
         <v>113</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1481,10 +1481,10 @@
         <v>96</v>
       </c>
       <c r="B60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C60" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1497,10 +1497,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>158</v>
+      </c>
+      <c r="C62" t="s">
         <v>159</v>
-      </c>
-      <c r="C62" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1538,7 +1538,7 @@
         <v>103</v>
       </c>
       <c r="B66" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C66" t="s">
         <v>104</v>
@@ -1557,7 +1557,7 @@
         <v>110</v>
       </c>
       <c r="B68" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C68" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
final edits for draft submission
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E38304-DC57-4F51-A0EC-28F83B803996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A69A03-58CC-45D1-9C00-CB87DEDE2CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="790" windowWidth="19420" windowHeight="11620" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,9 +498,6 @@
     <t>A collection of decisions regarding how tables, or datasets, will be organized and related to one another</t>
   </si>
   <si>
-    <t>data set, dataframe, spreadsheet, rectangular data, tabular data, table</t>
-  </si>
-  <si>
     <t>Data structure</t>
   </si>
   <si>
@@ -537,9 +534,6 @@
     <t>secondary data, administrative data, third-party data</t>
   </si>
   <si>
-    <t>non-public data; controlled data; managed access data</t>
-  </si>
-  <si>
     <t>Under the HIPAA Privacy Rule, a limited dataset is one in which 16 of the 18 HIPAA protected identifiers have been removed. Age, dates, and city/state/ZIP Code can remain. A limited dataset may be disclosed to external parties without authorization for specified purposes and often a data use agreement is required. This dataset is not considered de-identified and must be safeguarded against unauthorized access.</t>
   </si>
   <si>
@@ -562,6 +556,12 @@
   </si>
   <si>
     <t>File format</t>
+  </si>
+  <si>
+    <t>data set, data frame, spreadsheet, rectangular data, tabular data, table</t>
+  </si>
+  <si>
+    <t>non-public data, controlled data, managed access data</t>
   </si>
 </sst>
 </file>
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFDD66-17FF-4EA8-972E-A7EADB2C89E2}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +958,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>68</v>
@@ -1015,7 +1015,7 @@
         <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1069,10 +1069,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
         <v>152</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C19" t="s">
         <v>153</v>
@@ -1113,7 +1113,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="C20" t="s">
         <v>85</v>
@@ -1135,7 +1135,7 @@
         <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" t="s">
         <v>84</v>
@@ -1181,7 +1181,7 @@
         <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" t="s">
         <v>109</v>
@@ -1197,13 +1197,13 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,18 +1262,18 @@
         <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1281,7 +1281,7 @@
         <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C38" t="s">
         <v>101</v>
@@ -1292,10 +1292,10 @@
         <v>44</v>
       </c>
       <c r="B39" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" t="s">
         <v>163</v>
-      </c>
-      <c r="C39" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
         <v>143</v>
       </c>
       <c r="C43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1468,7 +1468,7 @@
         <v>107</v>
       </c>
       <c r="B58" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C58" t="s">
         <v>122</v>
@@ -1525,7 +1525,7 @@
         <v>46</v>
       </c>
       <c r="B64" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C64" t="s">
         <v>47</v>
@@ -1558,7 +1558,7 @@
         <v>140</v>
       </c>
       <c r="C67" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add all CRC and personal edits
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A69A03-58CC-45D1-9C00-CB87DEDE2CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14902F62-B899-4ED4-A733-061F3175138E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
@@ -339,9 +339,6 @@
     <t>A mechanism designed to collect original data (e.g., observation form, questionnaire, assessment)</t>
   </si>
   <si>
-    <t>In this book, I use the term measure broadly to refer to a collection of items used to measure an outcome (e.g., an existing scale, an existing academic assessment).</t>
-  </si>
-  <si>
     <t>The Health Insurance Portability and Accountability Act is a federal law covering the protection of sensitive health information.</t>
   </si>
   <si>
@@ -426,9 +423,6 @@
     <t>Human subject</t>
   </si>
   <si>
-    <t>The Common Rule (45 CFR 46) definition of a human subject is a living individual about whom an investigator conducting research obtains; 1) Data through intervention or interaction with the individual, or 2) identifiable private information.</t>
-  </si>
-  <si>
     <t>Data collected from a study where researchers are observing the effect of an intervention without manipulating who is exposed to the intervention.</t>
   </si>
   <si>
@@ -438,9 +432,6 @@
     <t>quasi-identifiers</t>
   </si>
   <si>
-    <t>These variables do not alone identify a particular individual (e.g., ethnicity, gender), but if combined with other information, they could be used to identify a participant</t>
-  </si>
-  <si>
     <t>Disclosure risk</t>
   </si>
   <si>
@@ -483,9 +474,6 @@
     <t>Normalize</t>
   </si>
   <si>
-    <t xml:space="preserve">In this book, the term normalize is used to refer to returning a value to its normal, or expected state </t>
-  </si>
-  <si>
     <t>Standardize</t>
   </si>
   <si>
@@ -537,9 +525,6 @@
     <t>Under the HIPAA Privacy Rule, a limited dataset is one in which 16 of the 18 HIPAA protected identifiers have been removed. Age, dates, and city/state/ZIP Code can remain. A limited dataset may be disclosed to external parties without authorization for specified purposes and often a data use agreement is required. This dataset is not considered de-identified and must be safeguarded against unauthorized access.</t>
   </si>
   <si>
-    <t>First hand data that are generated/collected by the research team as part of the research study.</t>
-  </si>
-  <si>
     <t>This is a unique numeric or alphanumeric identifier, assigned to every participant or site, and used to create confidential and de-identified data. These identifiers allow researchers to link data across time or measure.</t>
   </si>
   <si>
@@ -562,6 +547,21 @@
   </si>
   <si>
     <t>non-public data, controlled data, managed access data</t>
+  </si>
+  <si>
+    <t>The Common Rule (45 CFR 46) definition of a human subject is a living individual about whom an investigator conducting research obtains: 1) Data through intervention or interaction with the individual, or 2) identifiable private information.</t>
+  </si>
+  <si>
+    <t>These variables do not alone identify a particular individual (e.g., ethnicity, gender), but, if combined with other information, they could be used to identify a participant</t>
+  </si>
+  <si>
+    <t>In this book, I use the term "measure" broadly to refer to a collection of items used to measure an outcome (e.g., an existing scale, an existing academic assessment).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this book, the term "normalize" is used to refer to returning a value to its normal, or expected state </t>
+  </si>
+  <si>
+    <t>First-hand data that are generated/collected by the research team as part of the research study.</t>
   </si>
 </sst>
 </file>
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFDD66-17FF-4EA8-972E-A7EADB2C89E2}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,10 +947,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>68</v>
@@ -1001,13 +1001,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,7 +1015,7 @@
         <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
         <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -1058,21 +1058,21 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,13 +1099,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C20" t="s">
         <v>85</v>
@@ -1124,7 +1124,7 @@
         <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
         <v>64</v>
@@ -1135,7 +1135,7 @@
         <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
         <v>84</v>
@@ -1146,7 +1146,7 @@
         <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1162,10 +1162,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1181,10 +1181,10 @@
         <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1192,34 +1192,34 @@
         <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B29" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C29" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C31" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1227,7 +1227,7 @@
         <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1243,10 +1243,10 @@
         <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1259,21 +1259,21 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C36" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1281,10 +1281,10 @@
         <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1292,10 +1292,10 @@
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C39" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1308,10 +1308,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C41" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1319,18 +1319,18 @@
         <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C43" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1360,18 +1360,18 @@
         <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>138</v>
+      </c>
+      <c r="C47" t="s">
         <v>141</v>
-      </c>
-      <c r="C47" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1387,18 +1387,18 @@
         <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" t="s">
         <v>118</v>
-      </c>
-      <c r="B50" t="s">
-        <v>115</v>
-      </c>
-      <c r="C50" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,21 +1465,21 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1487,18 +1487,18 @@
         <v>93</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C61" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1506,7 +1506,7 @@
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
         <v>46</v>
       </c>
       <c r="B64" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C64" t="s">
         <v>47</v>
@@ -1536,7 +1536,7 @@
         <v>98</v>
       </c>
       <c r="B65" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C65" t="s">
         <v>99</v>
@@ -1552,13 +1552,13 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B67" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C67" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1566,7 +1566,7 @@
         <v>34</v>
       </c>
       <c r="B68" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C68" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
crc updates to additional chapters
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14902F62-B899-4ED4-A733-061F3175138E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BFF207-7B0B-4DD1-AF21-FA5EB9C5DC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18045" windowHeight="10620" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="175">
   <si>
     <t>Term</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Participant database</t>
   </si>
   <si>
-    <t>This database, or spreadsheet, includes any identifiable information on your participants as well as their assigned study ID. It is your only own means of linking your confidential research study data to a participant’s true identity. It is also used to track data collected across time and measures as well as participant attrition.</t>
-  </si>
-  <si>
     <t>Attrition</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>Numerical data that can be analyzed with statistical methods.</t>
   </si>
   <si>
-    <t>A study design that randomly assigns participants to a control or treatment condition. In education research you often hear about two types of RCTs. The first being the Individual-Level Randomized Controlled Trial (I-RCT) in which individuals (such as students) are randomized directly to the treatment or control group. The second is a Cluster Randomized Controlled Trial (C-RCT), sometimes also called group-randomized, in which clusters of students (such as classrooms) are randomized.</t>
-  </si>
-  <si>
     <t>Archive</t>
   </si>
   <si>
@@ -246,9 +240,6 @@
     <t>The transfer of data to a facility, such as a repository, that preserves and stores data long-term.</t>
   </si>
   <si>
-    <t>Data collected from a study where researchers randomly introduce an intervention and study the effects.</t>
-  </si>
-  <si>
     <t>A classification that specifies what types of values are contained in a variable and what kinds of operations can be performed on that variable. Examples of types include numeric, character, logical, or datetime.</t>
   </si>
   <si>
@@ -258,15 +249,6 @@
     <t>Research</t>
   </si>
   <si>
-    <t>measurement unit, variable format, variable class</t>
-  </si>
-  <si>
-    <t>Observational data</t>
-  </si>
-  <si>
-    <t>Experimental data</t>
-  </si>
-  <si>
     <t>Derived data</t>
   </si>
   <si>
@@ -291,15 +273,9 @@
     <t>Data created through transformations of existing data (e.g., mean scores).</t>
   </si>
   <si>
-    <t>A structured collection of data usually stored in tabular form. A research study usually produces one final dataset per entity/unit (e.g., teacher dataset, student dataset).</t>
-  </si>
-  <si>
     <t>Direct identifiers</t>
   </si>
   <si>
-    <t>file structure, file tree</t>
-  </si>
-  <si>
     <t>Indirect identifiers</t>
   </si>
   <si>
@@ -351,9 +327,6 @@
     <t>A single funded research project resulting in one or more datasets to be used to answer a research question.</t>
   </si>
   <si>
-    <t>Limited data set</t>
-  </si>
-  <si>
     <t>Restricted-use data</t>
   </si>
   <si>
@@ -423,9 +396,6 @@
     <t>Human subject</t>
   </si>
   <si>
-    <t>Data collected from a study where researchers are observing the effect of an intervention without manipulating who is exposed to the intervention.</t>
-  </si>
-  <si>
     <t>Confidentiality concerns data, ensuring participants agree to how their private and identifiable information will be managed and disseminated.</t>
   </si>
   <si>
@@ -483,9 +453,6 @@
     <t>Database design</t>
   </si>
   <si>
-    <t>A collection of decisions regarding how tables, or datasets, will be organized and related to one another</t>
-  </si>
-  <si>
     <t>Data structure</t>
   </si>
   <si>
@@ -507,9 +474,6 @@
     <t>calculated values</t>
   </si>
   <si>
-    <t>vertical join, join columns</t>
-  </si>
-  <si>
     <t>horizontal join, join rows, link</t>
   </si>
   <si>
@@ -519,12 +483,6 @@
     <t>A way that information is encoded for storage on a computer. There are both proprietary (e.g., SPSS, XLSX) and non-proprietary formats (e.g., CSV, TXT).</t>
   </si>
   <si>
-    <t>secondary data, administrative data, third-party data</t>
-  </si>
-  <si>
-    <t>Under the HIPAA Privacy Rule, a limited dataset is one in which 16 of the 18 HIPAA protected identifiers have been removed. Age, dates, and city/state/ZIP Code can remain. A limited dataset may be disclosed to external parties without authorization for specified purposes and often a data use agreement is required. This dataset is not considered de-identified and must be safeguarded against unauthorized access.</t>
-  </si>
-  <si>
     <t>This is a unique numeric or alphanumeric identifier, assigned to every participant or site, and used to create confidential and de-identified data. These identifiers allow researchers to link data across time or measure.</t>
   </si>
   <si>
@@ -558,10 +516,49 @@
     <t>In this book, I use the term "measure" broadly to refer to a collection of items used to measure an outcome (e.g., an existing scale, an existing academic assessment).</t>
   </si>
   <si>
-    <t xml:space="preserve">In this book, the term "normalize" is used to refer to returning a value to its normal, or expected state </t>
-  </si>
-  <si>
     <t>First-hand data that are generated/collected by the research team as part of the research study.</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Data providing details about other data.</t>
+  </si>
+  <si>
+    <t>vertical join, join columns, union</t>
+  </si>
+  <si>
+    <t>measurement unit, variable format, variable class, variable type</t>
+  </si>
+  <si>
+    <t>A collection of decisions regarding how tables, or datasets, will be organized and related to one another.</t>
+  </si>
+  <si>
+    <t>A structured collection of data usually stored in tabular form. A research study may produce one final dataset per entity/unit (e.g., teacher dataset, student dataset).</t>
+  </si>
+  <si>
+    <t>file structure, file tree, folder structure</t>
+  </si>
+  <si>
+    <t>secondary data, administrative data, third-party data, external data</t>
+  </si>
+  <si>
+    <t>This database, or spreadsheet, includes any identifiable information on your participants as well as their assigned study ID. It is your only means of linking your confidential research study data to a participant’s true identity. It is also used to track data collected across time and measures as well as participant attrition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A study design that randomly assigns participants, or groups of participants, to a control or treatment condition. </t>
+  </si>
+  <si>
+    <t>In this book, the term "normalize" is used to refer to returning a value to its normal, or expected state.</t>
+  </si>
+  <si>
+    <t>Persistent identifier</t>
+  </si>
+  <si>
+    <t>PID</t>
+  </si>
+  <si>
+    <t>A unique and enduring digital reference to an object, contributor, or organization. A DOI (digital object identifier) is a type of PID specific to digital objects.</t>
   </si>
 </sst>
 </file>
@@ -913,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DFDD66-17FF-4EA8-972E-A7EADB2C89E2}">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,56 +936,56 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1001,29 +998,29 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1031,7 +1028,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -1039,366 +1036,369 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
         <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>167</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>168</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" t="s">
-        <v>161</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>154</v>
+      </c>
+      <c r="B28" t="s">
+        <v>153</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>168</v>
-      </c>
-      <c r="B29" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="C29" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>80</v>
+      </c>
+      <c r="B33" t="s">
+        <v>121</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>172</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>144</v>
+      </c>
+      <c r="B35" t="s">
+        <v>141</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>151</v>
       </c>
       <c r="C36" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>155</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C37" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" t="s">
-        <v>158</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>159</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>135</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>129</v>
+      </c>
+      <c r="B41" t="s">
+        <v>130</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>17</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>139</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>140</v>
+        <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>175</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>172</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C46" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>59</v>
       </c>
       <c r="C47" t="s">
-        <v>141</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>108</v>
+      </c>
+      <c r="B49" t="s">
+        <v>105</v>
       </c>
       <c r="C49" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>117</v>
-      </c>
-      <c r="B50" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1406,42 +1406,42 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>73</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C55" t="s">
         <v>52</v>
@@ -1449,154 +1449,146 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C56" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>97</v>
+      </c>
+      <c r="B57" t="s">
+        <v>156</v>
       </c>
       <c r="C57" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>106</v>
-      </c>
-      <c r="B58" t="s">
-        <v>170</v>
+        <v>107</v>
       </c>
       <c r="C58" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>85</v>
+      </c>
+      <c r="B59" t="s">
+        <v>113</v>
       </c>
       <c r="C59" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>93</v>
-      </c>
-      <c r="B60" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C60" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>146</v>
+        <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="C64" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>98</v>
-      </c>
-      <c r="B65" t="s">
-        <v>144</v>
+        <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>95</v>
+      </c>
+      <c r="B66" t="s">
+        <v>127</v>
       </c>
       <c r="C66" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="C67" t="s">
-        <v>163</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>36</v>
       </c>
       <c r="C68" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C69" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>10</v>
-      </c>
-      <c r="B70" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C70">
-    <sortCondition ref="A2:A70"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C69">
+    <sortCondition ref="A2:A69"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update small formatting issues
</commit_message>
<xml_diff>
--- a/img/def_table.xlsx
+++ b/img/def_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Documents\data-mgmt-ed-research-book\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BFF207-7B0B-4DD1-AF21-FA5EB9C5DC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3CB46A-7755-451B-9D57-74FCC18342EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18045" windowHeight="10620" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E0487D93-AE54-4416-82FD-B0493CA700D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -366,9 +366,6 @@
     <t>The HIPAA Privacy Rule provides protections for 18  identifiers held by covered entities providing health care services.</t>
   </si>
   <si>
-    <t>Under the HIPAA Privacy Rule, there are two methods of de-identification. The Safe Harbor method allows covered entities to treat data as de-identified if all 18 PHI variables are removed.</t>
-  </si>
-  <si>
     <t>An umbrella term that encompasses proprietary, ethical, contractual, or private information that should be protected from unwarranted disclosure. There are varying levels of data sensitivity.</t>
   </si>
   <si>
@@ -559,6 +556,9 @@
   </si>
   <si>
     <t>A unique and enduring digital reference to an object, contributor, or organization. A DOI (digital object identifier) is a type of PID specific to digital objects.</t>
+  </si>
+  <si>
+    <t>Under the HIPAA Privacy Rule, there are two methods of de-identification. The safe harbor method allows covered entities to treat data as de-identified if all 18 PHI variables are removed.</t>
   </si>
 </sst>
 </file>
@@ -913,17 +913,17 @@
   <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
+    <col min="2" max="2" width="39.26953125" customWidth="1"/>
+    <col min="3" max="3" width="35.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -934,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -942,26 +942,26 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -969,7 +969,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -977,7 +977,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -988,7 +988,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -996,34 +996,34 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1053,37 +1053,37 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" t="s">
         <v>124</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>125</v>
       </c>
-      <c r="C15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1094,29 +1094,29 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -1127,18 +1127,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -1146,37 +1146,37 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" t="s">
         <v>122</v>
       </c>
-      <c r="C25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -1184,34 +1184,34 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C28" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" t="s">
         <v>132</v>
       </c>
-      <c r="C29" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -1227,18 +1227,18 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>80</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -1246,48 +1246,48 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C36" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>43</v>
       </c>
       <c r="B37" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" t="s">
         <v>146</v>
       </c>
-      <c r="C37" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" t="s">
         <v>161</v>
       </c>
-      <c r="C38" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1295,26 +1295,26 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" t="s">
         <v>129</v>
       </c>
-      <c r="B41" t="s">
-        <v>130</v>
-      </c>
       <c r="C41" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1322,10 +1322,10 @@
         <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1336,18 +1336,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" t="s">
         <v>172</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>173</v>
       </c>
-      <c r="C44" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -1355,18 +1355,18 @@
         <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -1374,15 +1374,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>73</v>
       </c>
@@ -1417,10 +1417,10 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -1455,45 +1455,45 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>97</v>
       </c>
       <c r="B57" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C57" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>107</v>
       </c>
       <c r="C58" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>85</v>
       </c>
       <c r="B59" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" t="s">
         <v>136</v>
       </c>
-      <c r="C60" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>3</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -1512,29 +1512,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C63" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C64" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>13</v>
       </c>
@@ -1542,18 +1542,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>95</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C66" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>33</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>35</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>10</v>
       </c>

</xml_diff>